<commit_message>
edit send email with solution
</commit_message>
<xml_diff>
--- a/src/EmailMaketing.Web/wwwroot/FilesUpload/SenderEmails 1 (3).xlsx
+++ b/src/EmailMaketing.Web/wwwroot/FilesUpload/SenderEmails 1 (3).xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25423"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25425"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E80634F-60A3-4245-9CF7-8A2D62303FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{381E9FF4-F541-4B5B-AAB8-3B5FD581FE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>